<commit_message>
Updates from CGIT, changes applied
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@1272 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/ballots/2013-05 QA Review/FHIR May Results.xlsx
+++ b/ballots/2013-05 QA Review/FHIR May Results.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Review Comments'!$B$1:$H$614</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Review Comments'!$B$1:$H$615</definedName>
     <definedName name="Resources">#REF!</definedName>
     <definedName name="Topics">#REF!</definedName>
   </definedNames>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4299" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4310" uniqueCount="931">
   <si>
     <t>Resource</t>
   </si>
@@ -3145,16 +3145,10 @@
     <t>Have already agreed to move first paragraph up.  The primary purpose of the Conformance statement is to just define the interface, not the behavior behind the scenes.  So it should cover "list of interfaces", but not architecture diagram - though you could certainly add the latter as an extension :&gt;</t>
   </si>
   <si>
-    <t>Will reword to "Profiles of each of these 3 types can be used together" to help avoid confusion.  (Each profile has a single type, but you can have all 3 types of profiles playing together.)</t>
-  </si>
-  <si>
     <t>Determined by the code - value sets are orthogonal</t>
   </si>
   <si>
     <t>Will be handled by exposing explicit path.</t>
-  </si>
-  <si>
-    <t>Correct the enumeration of group types.</t>
   </si>
   <si>
     <t>See above</t>
@@ -3167,21 +3161,9 @@
     <t>If not sure, click through to the full definition.  (The "how to read" section will identify the fact you can do this)</t>
   </si>
   <si>
-    <t>Will add Quantity as a type for characteristic.value</t>
-  </si>
-  <si>
-    <t>Will make characteristics.exclude 1..1</t>
-  </si>
-  <si>
-    <t>Well, for animals, you can use code to distinguish chickens, cows, etc. (even specific breeds or strains).  I'm not aware of any similar coding system for people.  However, it's not a "firm" prohibition, so will move it to a note and remove it from constraint.</t>
-  </si>
-  <si>
     <t>Should we rename "IssueReport" to "SystemIssueReport"?</t>
   </si>
   <si>
-    <t>Will add "description"</t>
-  </si>
-  <si>
     <t>Will change to "IssueReport resources"</t>
   </si>
   <si>
@@ -3219,10 +3201,6 @@
   </si>
   <si>
     <t>Will institute a QA process that flags all paragraphs containing "should", "shall", "must", "may", "might", "can" and allows for human review.  Will also provide a style guide of what terms to use for conformance criteria assertions, such as whether conformance labeling should be made for non-testable assertions.</t>
-  </si>
-  <si>
-    <t>Will add a constraint that, if members and quantity are both present, number of members can't be more than quantity.  Will also add a note that says that if the quantity is greater than the number of members, that means that the set of listed members is not complete.
-There's lots of value in having a group that doesn't list members.  E.g. "All people within 2 miles of point X" or "females aged 40-65".</t>
   </si>
   <si>
     <t>Will change these phrases to be in quotes and add more descriptive text:
@@ -3632,13 +3610,55 @@
   </si>
   <si>
     <t>Is it inside the 80% to search for procedures performed by a particular person?</t>
+  </si>
+  <si>
+    <t>Pub tooling</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Will add a constraint that, if members and quantity are both present, number of members can't be more than quantity.  Will also add a note that says that if the quantity is greater than the number of members, that means that the set of listed members is not complete.
+There's lots of value in having a group that doesn't list members.  E.g. "All people within 2 miles of point X" or "females aged 40-65".
+Done</t>
+  </si>
+  <si>
+    <t>Correct the enumeration of group types.
+Done</t>
+  </si>
+  <si>
+    <t>Will add Quantity as a type for characteristic.value
+Done</t>
+  </si>
+  <si>
+    <t>Will make characteristics.exclude 1..1
+Done</t>
+  </si>
+  <si>
+    <t>Well, for animals, you can use code to distinguish chickens, cows, etc. (even specific breeds or strains).  I'm not aware of any similar coding system for people.  However, it's not a "firm" prohibition, so will move it to a note and remove it from constraint.
+Done</t>
+  </si>
+  <si>
+    <t>The text (HTML rendering) should address this.  Will try to make this clear in the examples.</t>
+  </si>
+  <si>
+    <t>Rename "batch" to "transaction"</t>
+  </si>
+  <si>
+    <t>Will reword to "Profiles of each of these 3 types can be used together" to help avoid confusion.  (Each profile has a single type, but you can have all 3 types of profiles playing together.)  Will also provide an explicit example of how they can be used together.</t>
+  </si>
+  <si>
+    <t>Both (plus messaging request &amp; response).  Will make this clear by exposing explicit paths.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"batch" doesn't properly reflect </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3722,6 +3742,14 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -3755,13 +3783,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3853,10 +3882,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -4157,7 +4190,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I614"/>
+  <dimension ref="A1:I615"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
@@ -4364,7 +4397,7 @@
         <v>742</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>899</v>
+        <v>892</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>352</v>
@@ -4419,7 +4452,9 @@
       <c r="F9" s="12" t="s">
         <v>744</v>
       </c>
-      <c r="G9" s="22"/>
+      <c r="G9" s="22" t="s">
+        <v>919</v>
+      </c>
       <c r="H9" s="2" t="s">
         <v>547</v>
       </c>
@@ -4472,7 +4507,9 @@
       <c r="F11" s="11" t="s">
         <v>746</v>
       </c>
-      <c r="G11" s="21"/>
+      <c r="G11" s="22" t="s">
+        <v>919</v>
+      </c>
       <c r="H11" s="2" t="s">
         <v>120</v>
       </c>
@@ -4526,7 +4563,9 @@
       <c r="F13" s="11" t="s">
         <v>748</v>
       </c>
-      <c r="G13" s="21"/>
+      <c r="G13" s="22" t="s">
+        <v>919</v>
+      </c>
       <c r="H13" s="2" t="s">
         <v>407</v>
       </c>
@@ -4580,7 +4619,7 @@
         <v>750</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>900</v>
+        <v>893</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>54</v>
@@ -4609,7 +4648,7 @@
         <v>751</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>900</v>
+        <v>893</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>54</v>
@@ -4638,7 +4677,7 @@
         <v>752</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>899</v>
+        <v>892</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>547</v>
@@ -4666,7 +4705,9 @@
       <c r="F18" s="11" t="s">
         <v>753</v>
       </c>
-      <c r="G18" s="21"/>
+      <c r="G18" s="22" t="s">
+        <v>919</v>
+      </c>
       <c r="H18" s="2" t="s">
         <v>416</v>
       </c>
@@ -4746,7 +4787,7 @@
         <v>759</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>900</v>
+        <v>893</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>416</v>
@@ -4799,7 +4840,7 @@
         <v>483</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="G23" s="21"/>
       <c r="H23" s="2" t="s">
@@ -4934,7 +4975,9 @@
       <c r="F28" s="14" t="s">
         <v>764</v>
       </c>
-      <c r="G28" s="26"/>
+      <c r="G28" s="26" t="s">
+        <v>920</v>
+      </c>
       <c r="H28" s="2" t="s">
         <v>369</v>
       </c>
@@ -4984,8 +5027,8 @@
       <c r="E30" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>766</v>
+      <c r="F30" s="11" t="s">
+        <v>928</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>248</v>
@@ -5011,7 +5054,7 @@
         <v>485</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>416</v>
@@ -5037,7 +5080,7 @@
         <v>484</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>768</v>
+        <v>929</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>416</v>
@@ -5063,7 +5106,7 @@
         <v>486</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>416</v>
@@ -5072,7 +5115,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -5089,7 +5132,7 @@
         <v>64</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>791</v>
+        <v>921</v>
       </c>
       <c r="G34" s="21"/>
       <c r="H34" s="2" t="s">
@@ -5143,7 +5186,7 @@
         <v>489</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>769</v>
+        <v>922</v>
       </c>
       <c r="G36" s="21"/>
       <c r="H36" s="2" t="s">
@@ -5170,7 +5213,7 @@
         <v>487</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>352</v>
@@ -5196,7 +5239,7 @@
         <v>488</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>773</v>
+        <v>923</v>
       </c>
       <c r="G38" s="21"/>
       <c r="H38" s="2" t="s">
@@ -5223,7 +5266,7 @@
         <v>490</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>774</v>
+        <v>924</v>
       </c>
       <c r="G39" s="21"/>
       <c r="H39" s="2" t="s">
@@ -5233,7 +5276,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -5250,7 +5293,7 @@
         <v>155</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>775</v>
+        <v>925</v>
       </c>
       <c r="G40" s="21"/>
       <c r="H40" s="2" t="s">
@@ -5277,7 +5320,7 @@
         <v>417</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>416</v>
@@ -5303,10 +5346,10 @@
         <v>68</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>900</v>
+        <v>893</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>59</v>
@@ -5358,8 +5401,8 @@
       <c r="E44" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="F44" s="11" t="s">
-        <v>777</v>
+      <c r="F44" s="17" t="s">
+        <v>926</v>
       </c>
       <c r="G44" s="21"/>
       <c r="H44" s="2" t="s">
@@ -5386,7 +5429,7 @@
         <v>161</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
       <c r="G45" s="21"/>
       <c r="H45" s="2" t="s">
@@ -5413,7 +5456,7 @@
         <v>162</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="G46" s="21"/>
       <c r="H46" s="2" t="s">
@@ -5440,7 +5483,7 @@
         <v>271</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="G47" s="19"/>
       <c r="H47" s="2" t="s">
@@ -5467,7 +5510,7 @@
         <v>321</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
       <c r="G48" s="21"/>
       <c r="H48" s="2" t="s">
@@ -5494,7 +5537,7 @@
         <v>447</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>811</v>
+        <v>804</v>
       </c>
       <c r="G49" s="21"/>
       <c r="H49" s="2" t="s">
@@ -5521,7 +5564,7 @@
         <v>418</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>812</v>
+        <v>805</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>416</v>
@@ -5573,7 +5616,7 @@
         <v>514</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="G52" s="21"/>
       <c r="H52" s="2" t="s">
@@ -5600,7 +5643,7 @@
         <v>513</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="G53" s="21"/>
       <c r="H53" s="2" t="s">
@@ -5627,7 +5670,7 @@
         <v>163</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="G54" s="21"/>
       <c r="H54" s="2" t="s">
@@ -5654,7 +5697,7 @@
         <v>492</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="G55" s="21"/>
       <c r="H55" s="2" t="s">
@@ -5681,7 +5724,7 @@
         <v>71</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
       <c r="G56" s="21"/>
       <c r="H56" s="2" t="s">
@@ -5737,7 +5780,7 @@
         <v>725</v>
       </c>
       <c r="G58" s="20" t="s">
-        <v>900</v>
+        <v>893</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>85</v>
@@ -5790,10 +5833,10 @@
         <v>515</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="G60" s="20" t="s">
-        <v>901</v>
+        <v>894</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>352</v>
@@ -5819,7 +5862,7 @@
         <v>516</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="G61" s="21"/>
       <c r="H61" s="2" t="s">
@@ -5846,7 +5889,7 @@
         <v>167</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="G62" s="21"/>
       <c r="H62" s="2" t="s">
@@ -5873,10 +5916,10 @@
         <v>168</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
       <c r="G63" s="20" t="s">
-        <v>899</v>
+        <v>892</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>120</v>
@@ -5902,10 +5945,10 @@
         <v>169</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>792</v>
+        <v>785</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>902</v>
+        <v>895</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>120</v>
@@ -5931,10 +5974,10 @@
         <v>170</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>793</v>
+        <v>786</v>
       </c>
       <c r="G65" s="20" t="s">
-        <v>901</v>
+        <v>894</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>120</v>
@@ -5960,7 +6003,7 @@
         <v>269</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>794</v>
+        <v>787</v>
       </c>
       <c r="G66" s="19"/>
       <c r="H66" s="2" t="s">
@@ -5987,7 +6030,7 @@
         <v>418</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>810</v>
+        <v>803</v>
       </c>
       <c r="G67" s="21"/>
       <c r="H67" s="2" t="s">
@@ -6041,10 +6084,10 @@
         <v>208</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>795</v>
+        <v>788</v>
       </c>
       <c r="G69" s="20" t="s">
-        <v>903</v>
+        <v>896</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>120</v>
@@ -6070,7 +6113,7 @@
         <v>209</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>797</v>
+        <v>790</v>
       </c>
       <c r="G70" s="21"/>
       <c r="H70" s="2" t="s">
@@ -6097,7 +6140,7 @@
         <v>210</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>797</v>
+        <v>790</v>
       </c>
       <c r="G71" s="21"/>
       <c r="H71" s="2" t="s">
@@ -6124,7 +6167,7 @@
         <v>211</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>798</v>
+        <v>791</v>
       </c>
       <c r="G72" s="21"/>
       <c r="H72" s="2" t="s">
@@ -6151,7 +6194,7 @@
         <v>212</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>800</v>
+        <v>793</v>
       </c>
       <c r="G73" s="21"/>
       <c r="H73" s="2" t="s">
@@ -6178,7 +6221,7 @@
         <v>459</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>801</v>
+        <v>794</v>
       </c>
       <c r="G74" s="21"/>
       <c r="H74" s="2" t="s">
@@ -6205,7 +6248,7 @@
         <v>517</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>802</v>
+        <v>795</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>416</v>
@@ -6231,7 +6274,7 @@
         <v>518</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>802</v>
+        <v>795</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>416</v>
@@ -6257,7 +6300,7 @@
         <v>682</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G77" s="20" t="s">
         <v>470</v>
@@ -6286,7 +6329,7 @@
         <v>687</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G78" s="20" t="s">
         <v>470</v>
@@ -6318,7 +6361,7 @@
         <v>728</v>
       </c>
       <c r="G79" s="20" t="s">
-        <v>905</v>
+        <v>898</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>85</v>
@@ -6396,7 +6439,7 @@
         <v>424</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G82" s="20" t="s">
         <v>470</v>
@@ -6425,7 +6468,7 @@
         <v>683</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G83" s="21"/>
       <c r="H83" s="2" t="s">
@@ -6452,7 +6495,7 @@
         <v>684</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G84" s="21"/>
       <c r="H84" s="2" t="s">
@@ -6479,7 +6522,7 @@
         <v>686</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G85" s="20" t="s">
         <v>470</v>
@@ -6508,7 +6551,7 @@
         <v>688</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>886</v>
+        <v>879</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>547</v>
@@ -6534,7 +6577,7 @@
         <v>685</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>885</v>
+        <v>878</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>547</v>
@@ -6560,7 +6603,7 @@
         <v>382</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G88" s="28" t="s">
         <v>470</v>
@@ -6589,7 +6632,7 @@
         <v>383</v>
       </c>
       <c r="F89" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G89" s="26"/>
       <c r="H89" s="2" t="s">
@@ -6616,7 +6659,7 @@
         <v>384</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G90" s="26"/>
       <c r="H90" s="2" t="s">
@@ -6643,7 +6686,7 @@
         <v>385</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G91" s="26"/>
       <c r="H91" s="2" t="s">
@@ -6670,7 +6713,7 @@
         <v>386</v>
       </c>
       <c r="F92" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G92" s="26"/>
       <c r="H92" s="2" t="s">
@@ -6697,7 +6740,7 @@
         <v>214</v>
       </c>
       <c r="F93" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G93" s="21"/>
       <c r="H93" s="2" t="s">
@@ -6724,7 +6767,7 @@
         <v>215</v>
       </c>
       <c r="F94" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G94" s="21"/>
       <c r="H94" s="2" t="s">
@@ -6751,7 +6794,7 @@
         <v>216</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G95" s="21"/>
       <c r="H95" s="2" t="s">
@@ -6778,7 +6821,7 @@
         <v>217</v>
       </c>
       <c r="F96" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G96" s="21"/>
       <c r="H96" s="2" t="s">
@@ -6805,7 +6848,7 @@
         <v>218</v>
       </c>
       <c r="F97" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G97" s="21"/>
       <c r="H97" s="2" t="s">
@@ -6832,7 +6875,7 @@
         <v>219</v>
       </c>
       <c r="F98" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G98" s="21"/>
       <c r="H98" s="2" t="s">
@@ -6859,7 +6902,7 @@
         <v>220</v>
       </c>
       <c r="F99" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G99" s="21"/>
       <c r="H99" s="2" t="s">
@@ -6886,7 +6929,7 @@
         <v>221</v>
       </c>
       <c r="F100" s="11" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G100" s="21"/>
       <c r="H100" s="2" t="s">
@@ -6913,7 +6956,7 @@
         <v>222</v>
       </c>
       <c r="F101" s="9" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G101" s="20" t="s">
         <v>470</v>
@@ -6942,7 +6985,7 @@
         <v>681</v>
       </c>
       <c r="F102" s="9" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="G102" s="20" t="s">
         <v>470</v>
@@ -6971,7 +7014,7 @@
         <v>462</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>882</v>
+        <v>875</v>
       </c>
       <c r="H103" s="2" t="s">
         <v>429</v>
@@ -6997,7 +7040,7 @@
         <v>519</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>883</v>
+        <v>876</v>
       </c>
       <c r="H104" s="2" t="s">
         <v>416</v>
@@ -7023,7 +7066,7 @@
         <v>520</v>
       </c>
       <c r="F105" s="11" t="s">
-        <v>884</v>
+        <v>877</v>
       </c>
       <c r="G105" s="21"/>
       <c r="H105" s="2" t="s">
@@ -7077,7 +7120,7 @@
         <v>599</v>
       </c>
       <c r="F107" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G107" s="21"/>
       <c r="H107" s="2" t="s">
@@ -7104,10 +7147,10 @@
         <v>600</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>888</v>
+        <v>881</v>
       </c>
       <c r="G108" s="20" t="s">
-        <v>906</v>
+        <v>899</v>
       </c>
       <c r="H108" s="2" t="s">
         <v>352</v>
@@ -7133,7 +7176,7 @@
         <v>583</v>
       </c>
       <c r="F109" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G109" s="21"/>
       <c r="H109" s="2" t="s">
@@ -7160,7 +7203,7 @@
         <v>587</v>
       </c>
       <c r="F110" s="11" t="s">
-        <v>889</v>
+        <v>882</v>
       </c>
       <c r="G110" s="21"/>
       <c r="H110" s="2" t="s">
@@ -7187,7 +7230,7 @@
         <v>405</v>
       </c>
       <c r="F111" s="14" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G111" s="26"/>
       <c r="H111" s="2" t="s">
@@ -7214,7 +7257,7 @@
         <v>137</v>
       </c>
       <c r="F112" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G112" s="21"/>
       <c r="H112" s="2" t="s">
@@ -7241,7 +7284,7 @@
         <v>138</v>
       </c>
       <c r="F113" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G113" s="21"/>
       <c r="H113" s="2" t="s">
@@ -7268,7 +7311,7 @@
         <v>139</v>
       </c>
       <c r="F114" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G114" s="21"/>
       <c r="H114" s="2" t="s">
@@ -7295,10 +7338,10 @@
         <v>590</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>907</v>
+        <v>900</v>
       </c>
       <c r="G115" s="20" t="s">
-        <v>908</v>
+        <v>901</v>
       </c>
       <c r="H115" s="2" t="s">
         <v>547</v>
@@ -7324,7 +7367,7 @@
         <v>582</v>
       </c>
       <c r="F116" s="11" t="s">
-        <v>890</v>
+        <v>883</v>
       </c>
       <c r="G116" s="21"/>
       <c r="H116" s="2" t="s">
@@ -7351,7 +7394,7 @@
         <v>585</v>
       </c>
       <c r="F117" s="11" t="s">
-        <v>891</v>
+        <v>884</v>
       </c>
       <c r="G117" s="21"/>
       <c r="H117" s="2" t="s">
@@ -7378,7 +7421,7 @@
         <v>584</v>
       </c>
       <c r="F118" s="11" t="s">
-        <v>892</v>
+        <v>885</v>
       </c>
       <c r="G118" s="21"/>
       <c r="H118" s="2" t="s">
@@ -7405,7 +7448,7 @@
         <v>436</v>
       </c>
       <c r="F119" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G119" s="21"/>
       <c r="H119" s="2" t="s">
@@ -7432,7 +7475,7 @@
         <v>437</v>
       </c>
       <c r="F120" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G120" s="21"/>
       <c r="H120" s="2" t="s">
@@ -7459,7 +7502,7 @@
         <v>493</v>
       </c>
       <c r="F121" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G121" s="21"/>
       <c r="H121" s="2" t="s">
@@ -7486,7 +7529,7 @@
         <v>586</v>
       </c>
       <c r="F122" s="11" t="s">
-        <v>893</v>
+        <v>886</v>
       </c>
       <c r="G122" s="21"/>
       <c r="H122" s="2" t="s">
@@ -7542,7 +7585,7 @@
         <v>245</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>894</v>
+        <v>887</v>
       </c>
       <c r="G124" s="20" t="s">
         <v>8</v>
@@ -7571,7 +7614,7 @@
         <v>361</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>895</v>
+        <v>888</v>
       </c>
       <c r="G125" s="20" t="s">
         <v>8</v>
@@ -7600,7 +7643,7 @@
         <v>404</v>
       </c>
       <c r="F126" s="13" t="s">
-        <v>896</v>
+        <v>889</v>
       </c>
       <c r="G126" s="25"/>
       <c r="H126" s="2" t="s">
@@ -7627,7 +7670,7 @@
         <v>140</v>
       </c>
       <c r="F127" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G127" s="21"/>
       <c r="H127" s="2" t="s">
@@ -7654,7 +7697,7 @@
         <v>141</v>
       </c>
       <c r="F128" s="11" t="s">
-        <v>897</v>
+        <v>890</v>
       </c>
       <c r="G128" s="21"/>
       <c r="H128" s="2" t="s">
@@ -7681,7 +7724,7 @@
         <v>142</v>
       </c>
       <c r="F129" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G129" s="21"/>
       <c r="H129" s="2" t="s">
@@ -7708,7 +7751,7 @@
         <v>143</v>
       </c>
       <c r="F130" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G130" s="21"/>
       <c r="H130" s="2" t="s">
@@ -7735,7 +7778,7 @@
         <v>258</v>
       </c>
       <c r="F131" s="11" t="s">
-        <v>898</v>
+        <v>891</v>
       </c>
       <c r="G131" s="21"/>
       <c r="H131" s="2" t="s">
@@ -7762,7 +7805,7 @@
         <v>588</v>
       </c>
       <c r="F132" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="G132" s="21"/>
       <c r="H132" s="2" t="s">
@@ -7789,7 +7832,7 @@
         <v>438</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="G133" s="21"/>
       <c r="H133" s="2" t="s">
@@ -7887,7 +7930,7 @@
         <v>144</v>
       </c>
       <c r="F137" s="11" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="G137" s="21"/>
       <c r="H137" s="2" t="s">
@@ -8104,7 +8147,7 @@
         <v>495</v>
       </c>
       <c r="F146" s="11" t="s">
-        <v>858</v>
+        <v>851</v>
       </c>
       <c r="G146" s="21"/>
       <c r="H146" s="2" t="s">
@@ -8181,7 +8224,7 @@
         <v>156</v>
       </c>
       <c r="F149" s="11" t="s">
-        <v>859</v>
+        <v>852</v>
       </c>
       <c r="G149" s="21"/>
       <c r="H149" s="2" t="s">
@@ -8208,7 +8251,7 @@
         <v>157</v>
       </c>
       <c r="F150" s="11" t="s">
-        <v>860</v>
+        <v>853</v>
       </c>
       <c r="G150" s="21"/>
       <c r="H150" s="2" t="s">
@@ -8235,7 +8278,7 @@
         <v>158</v>
       </c>
       <c r="F151" s="11" t="s">
-        <v>861</v>
+        <v>854</v>
       </c>
       <c r="G151" s="21"/>
       <c r="H151" s="2" t="s">
@@ -8331,7 +8374,7 @@
         <v>310</v>
       </c>
       <c r="F155" s="11" t="s">
-        <v>862</v>
+        <v>855</v>
       </c>
       <c r="G155" s="21"/>
       <c r="H155" s="2" t="s">
@@ -8611,7 +8654,7 @@
         <v>445</v>
       </c>
       <c r="F167" s="11" t="s">
-        <v>863</v>
+        <v>856</v>
       </c>
       <c r="G167" s="21"/>
       <c r="H167" s="2" t="s">
@@ -8809,7 +8852,7 @@
         <v>735</v>
       </c>
       <c r="G175" s="20" t="s">
-        <v>905</v>
+        <v>898</v>
       </c>
       <c r="H175" s="2" t="s">
         <v>85</v>
@@ -8885,7 +8928,7 @@
         <v>388</v>
       </c>
       <c r="F178" s="14" t="s">
-        <v>864</v>
+        <v>857</v>
       </c>
       <c r="G178" s="26"/>
       <c r="H178" s="2" t="s">
@@ -9004,7 +9047,7 @@
         <v>524</v>
       </c>
       <c r="F183" s="11" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="G183" s="21"/>
       <c r="H183" s="2" t="s">
@@ -9031,7 +9074,7 @@
         <v>525</v>
       </c>
       <c r="F184" s="11" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="G184" s="21"/>
       <c r="H184" s="2" t="s">
@@ -9058,7 +9101,7 @@
         <v>526</v>
       </c>
       <c r="F185" s="11" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="G185" s="21"/>
       <c r="H185" s="2" t="s">
@@ -9225,7 +9268,7 @@
         <v>132</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>865</v>
+        <v>858</v>
       </c>
       <c r="H192" s="2" t="s">
         <v>120</v>
@@ -9416,7 +9459,7 @@
         <v>247</v>
       </c>
       <c r="F200" s="11" t="s">
-        <v>866</v>
+        <v>859</v>
       </c>
       <c r="G200" s="21"/>
       <c r="H200" s="2" t="s">
@@ -9608,7 +9651,7 @@
         <v>399</v>
       </c>
       <c r="F208" s="14" t="s">
-        <v>867</v>
+        <v>860</v>
       </c>
       <c r="G208" s="26"/>
       <c r="H208" s="2" t="s">
@@ -9635,7 +9678,7 @@
         <v>400</v>
       </c>
       <c r="F209" s="14" t="s">
-        <v>870</v>
+        <v>863</v>
       </c>
       <c r="G209" s="26"/>
       <c r="H209" s="2" t="s">
@@ -9662,7 +9705,7 @@
         <v>401</v>
       </c>
       <c r="F210" s="14" t="s">
-        <v>869</v>
+        <v>862</v>
       </c>
       <c r="G210" s="26"/>
       <c r="H210" s="2" t="s">
@@ -9689,7 +9732,7 @@
         <v>402</v>
       </c>
       <c r="F211" s="4" t="s">
-        <v>806</v>
+        <v>799</v>
       </c>
       <c r="G211" s="29"/>
       <c r="H211" s="2" t="s">
@@ -9785,7 +9828,7 @@
         <v>290</v>
       </c>
       <c r="F215" s="9" t="s">
-        <v>868</v>
+        <v>861</v>
       </c>
       <c r="G215" s="20" t="s">
         <v>470</v>
@@ -9952,7 +9995,7 @@
         <v>297</v>
       </c>
       <c r="F222" s="8" t="s">
-        <v>871</v>
+        <v>864</v>
       </c>
       <c r="G222" s="19"/>
       <c r="H222" s="2" t="s">
@@ -10232,7 +10275,7 @@
         <v>443</v>
       </c>
       <c r="F234" s="11" t="s">
-        <v>872</v>
+        <v>865</v>
       </c>
       <c r="G234" s="21"/>
       <c r="H234" s="2" t="s">
@@ -10282,7 +10325,7 @@
         <v>529</v>
       </c>
       <c r="F236" s="11" t="s">
-        <v>826</v>
+        <v>819</v>
       </c>
       <c r="G236" s="21"/>
       <c r="H236" s="2" t="s">
@@ -10335,7 +10378,7 @@
         <v>738</v>
       </c>
       <c r="G238" s="20" t="s">
-        <v>909</v>
+        <v>902</v>
       </c>
       <c r="H238" s="2" t="s">
         <v>85</v>
@@ -10430,7 +10473,7 @@
         <v>460</v>
       </c>
       <c r="F242" s="11" t="s">
-        <v>873</v>
+        <v>866</v>
       </c>
       <c r="G242" s="21"/>
       <c r="H242" s="2" t="s">
@@ -10457,7 +10500,7 @@
         <v>461</v>
       </c>
       <c r="F243" s="8" t="s">
-        <v>874</v>
+        <v>867</v>
       </c>
       <c r="G243" s="19"/>
       <c r="H243" s="2" t="s">
@@ -10507,7 +10550,7 @@
         <v>532</v>
       </c>
       <c r="F245" s="11" t="s">
-        <v>875</v>
+        <v>868</v>
       </c>
       <c r="G245" s="21"/>
       <c r="H245" s="2" t="s">
@@ -10560,10 +10603,10 @@
         <v>223</v>
       </c>
       <c r="F247" s="9" t="s">
-        <v>876</v>
+        <v>869</v>
       </c>
       <c r="G247" s="20" t="s">
-        <v>909</v>
+        <v>902</v>
       </c>
       <c r="H247" s="2" t="s">
         <v>120</v>
@@ -10635,7 +10678,7 @@
         <v>463</v>
       </c>
       <c r="F250" s="11" t="s">
-        <v>877</v>
+        <v>870</v>
       </c>
       <c r="G250" s="21"/>
       <c r="H250" s="2" t="s">
@@ -10662,7 +10705,7 @@
         <v>534</v>
       </c>
       <c r="F251" s="11" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="G251" s="21"/>
       <c r="H251" s="2" t="s">
@@ -10689,7 +10732,7 @@
         <v>533</v>
       </c>
       <c r="F252" s="11" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="G252" s="21"/>
       <c r="H252" s="2" t="s">
@@ -10739,10 +10782,10 @@
         <v>60</v>
       </c>
       <c r="F254" s="9" t="s">
-        <v>803</v>
+        <v>796</v>
       </c>
       <c r="G254" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H254" s="2" t="s">
         <v>59</v>
@@ -10794,7 +10837,7 @@
         <v>239</v>
       </c>
       <c r="F256" s="8" t="s">
-        <v>804</v>
+        <v>797</v>
       </c>
       <c r="G256" s="19"/>
       <c r="H256" s="2" t="s">
@@ -10821,7 +10864,7 @@
         <v>355</v>
       </c>
       <c r="F257" s="2" t="s">
-        <v>805</v>
+        <v>798</v>
       </c>
       <c r="H257" s="2" t="s">
         <v>352</v>
@@ -10847,7 +10890,7 @@
         <v>231</v>
       </c>
       <c r="F258" s="2" t="s">
-        <v>806</v>
+        <v>799</v>
       </c>
       <c r="H258" s="2" t="s">
         <v>230</v>
@@ -10873,7 +10916,7 @@
         <v>370</v>
       </c>
       <c r="F259" s="2" t="s">
-        <v>805</v>
+        <v>798</v>
       </c>
       <c r="H259" s="2" t="s">
         <v>369</v>
@@ -10899,7 +10942,7 @@
         <v>371</v>
       </c>
       <c r="F260" s="14" t="s">
-        <v>807</v>
+        <v>800</v>
       </c>
       <c r="G260" s="26"/>
       <c r="H260" s="2" t="s">
@@ -10926,7 +10969,7 @@
         <v>123</v>
       </c>
       <c r="F261" s="11" t="s">
-        <v>808</v>
+        <v>801</v>
       </c>
       <c r="G261" s="21"/>
       <c r="H261" s="2" t="s">
@@ -10953,7 +10996,7 @@
         <v>124</v>
       </c>
       <c r="F262" s="11" t="s">
-        <v>809</v>
+        <v>802</v>
       </c>
       <c r="G262" s="21"/>
       <c r="H262" s="2" t="s">
@@ -10980,10 +11023,10 @@
         <v>249</v>
       </c>
       <c r="F263" s="9" t="s">
-        <v>813</v>
+        <v>806</v>
       </c>
       <c r="G263" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H263" s="2" t="s">
         <v>248</v>
@@ -11009,7 +11052,7 @@
         <v>250</v>
       </c>
       <c r="F264" s="2" t="s">
-        <v>814</v>
+        <v>807</v>
       </c>
       <c r="H264" s="2" t="s">
         <v>248</v>
@@ -11035,7 +11078,7 @@
         <v>408</v>
       </c>
       <c r="F265" s="11" t="s">
-        <v>815</v>
+        <v>808</v>
       </c>
       <c r="G265" s="21"/>
       <c r="H265" s="2" t="s">
@@ -11062,10 +11105,10 @@
         <v>276</v>
       </c>
       <c r="F266" s="9" t="s">
-        <v>816</v>
+        <v>809</v>
       </c>
       <c r="G266" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H266" s="2" t="s">
         <v>351</v>
@@ -11091,7 +11134,7 @@
         <v>277</v>
       </c>
       <c r="F267" s="11" t="s">
-        <v>817</v>
+        <v>810</v>
       </c>
       <c r="G267" s="21"/>
       <c r="H267" s="2" t="s">
@@ -11118,10 +11161,10 @@
         <v>278</v>
       </c>
       <c r="F268" s="9" t="s">
-        <v>816</v>
+        <v>809</v>
       </c>
       <c r="G268" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H268" s="2" t="s">
         <v>351</v>
@@ -11147,10 +11190,10 @@
         <v>279</v>
       </c>
       <c r="F269" s="9" t="s">
-        <v>818</v>
+        <v>811</v>
       </c>
       <c r="G269" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H269" s="2" t="s">
         <v>351</v>
@@ -11203,7 +11246,7 @@
         <v>431</v>
       </c>
       <c r="F271" s="2" t="s">
-        <v>819</v>
+        <v>812</v>
       </c>
       <c r="H271" s="2" t="s">
         <v>429</v>
@@ -11255,7 +11298,7 @@
         <v>232</v>
       </c>
       <c r="F273" s="2" t="s">
-        <v>806</v>
+        <v>799</v>
       </c>
       <c r="H273" s="2" t="s">
         <v>230</v>
@@ -11281,10 +11324,10 @@
         <v>372</v>
       </c>
       <c r="F274" s="15" t="s">
-        <v>820</v>
+        <v>813</v>
       </c>
       <c r="G274" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H274" s="2" t="s">
         <v>369</v>
@@ -11310,7 +11353,7 @@
         <v>373</v>
       </c>
       <c r="F275" s="4" t="s">
-        <v>821</v>
+        <v>814</v>
       </c>
       <c r="G275" s="29"/>
       <c r="H275" s="2" t="s">
@@ -11337,7 +11380,7 @@
         <v>125</v>
       </c>
       <c r="F276" s="11" t="s">
-        <v>822</v>
+        <v>815</v>
       </c>
       <c r="G276" s="21"/>
       <c r="H276" s="2" t="s">
@@ -11364,7 +11407,7 @@
         <v>126</v>
       </c>
       <c r="F277" s="11" t="s">
-        <v>823</v>
+        <v>816</v>
       </c>
       <c r="G277" s="21"/>
       <c r="H277" s="2" t="s">
@@ -11391,7 +11434,7 @@
         <v>251</v>
       </c>
       <c r="F278" s="8" t="s">
-        <v>824</v>
+        <v>817</v>
       </c>
       <c r="G278" s="19"/>
       <c r="H278" s="2" t="s">
@@ -11445,7 +11488,7 @@
         <v>433</v>
       </c>
       <c r="F280" s="11" t="s">
-        <v>825</v>
+        <v>818</v>
       </c>
       <c r="G280" s="21"/>
       <c r="H280" s="2" t="s">
@@ -11472,7 +11515,7 @@
         <v>496</v>
       </c>
       <c r="F281" s="11" t="s">
-        <v>826</v>
+        <v>819</v>
       </c>
       <c r="G281" s="21"/>
       <c r="H281" s="2" t="s">
@@ -11499,7 +11542,7 @@
         <v>61</v>
       </c>
       <c r="F282" s="8" t="s">
-        <v>828</v>
+        <v>821</v>
       </c>
       <c r="G282" s="19"/>
       <c r="H282" s="2" t="s">
@@ -11526,10 +11569,10 @@
         <v>241</v>
       </c>
       <c r="F283" s="9" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
       <c r="G283" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H283" s="2" t="s">
         <v>238</v>
@@ -11555,10 +11598,10 @@
         <v>357</v>
       </c>
       <c r="F284" s="9" t="s">
-        <v>830</v>
+        <v>823</v>
       </c>
       <c r="G284" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H284" s="2" t="s">
         <v>352</v>
@@ -11584,7 +11627,7 @@
         <v>374</v>
       </c>
       <c r="F285" s="14" t="s">
-        <v>831</v>
+        <v>824</v>
       </c>
       <c r="G285" s="26"/>
       <c r="H285" s="2" t="s">
@@ -11611,7 +11654,7 @@
         <v>375</v>
       </c>
       <c r="F286" s="4" t="s">
-        <v>832</v>
+        <v>825</v>
       </c>
       <c r="G286" s="29"/>
       <c r="H286" s="2" t="s">
@@ -11638,7 +11681,7 @@
         <v>376</v>
       </c>
       <c r="F287" s="14" t="s">
-        <v>833</v>
+        <v>826</v>
       </c>
       <c r="G287" s="26"/>
       <c r="H287" s="2" t="s">
@@ -11665,7 +11708,7 @@
         <v>127</v>
       </c>
       <c r="F288" s="11" t="s">
-        <v>834</v>
+        <v>827</v>
       </c>
       <c r="G288" s="21"/>
       <c r="H288" s="2" t="s">
@@ -11692,7 +11735,7 @@
         <v>128</v>
       </c>
       <c r="F289" s="11" t="s">
-        <v>835</v>
+        <v>828</v>
       </c>
       <c r="G289" s="21"/>
       <c r="H289" s="2" t="s">
@@ -11719,7 +11762,7 @@
         <v>129</v>
       </c>
       <c r="F290" s="11" t="s">
-        <v>831</v>
+        <v>824</v>
       </c>
       <c r="G290" s="21"/>
       <c r="H290" s="2" t="s">
@@ -11746,7 +11789,7 @@
         <v>130</v>
       </c>
       <c r="F291" s="11" t="s">
-        <v>836</v>
+        <v>829</v>
       </c>
       <c r="G291" s="21"/>
       <c r="H291" s="2" t="s">
@@ -11773,7 +11816,7 @@
         <v>409</v>
       </c>
       <c r="F292" s="2" t="s">
-        <v>837</v>
+        <v>830</v>
       </c>
       <c r="H292" s="2" t="s">
         <v>407</v>
@@ -11799,7 +11842,7 @@
         <v>434</v>
       </c>
       <c r="F293" s="11" t="s">
-        <v>838</v>
+        <v>831</v>
       </c>
       <c r="G293" s="21"/>
       <c r="H293" s="2" t="s">
@@ -11826,7 +11869,7 @@
         <v>497</v>
       </c>
       <c r="F294" s="2" t="s">
-        <v>839</v>
+        <v>832</v>
       </c>
       <c r="H294" s="2" t="s">
         <v>416</v>
@@ -11852,10 +11895,10 @@
         <v>621</v>
       </c>
       <c r="F295" s="9" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="G295" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H295" s="2" t="s">
         <v>547</v>
@@ -11881,10 +11924,10 @@
         <v>363</v>
       </c>
       <c r="F296" s="9" t="s">
-        <v>840</v>
+        <v>833</v>
       </c>
       <c r="G296" s="20" t="s">
-        <v>910</v>
+        <v>903</v>
       </c>
       <c r="H296" s="2" t="s">
         <v>352</v>
@@ -11910,10 +11953,10 @@
         <v>620</v>
       </c>
       <c r="F297" s="9" t="s">
-        <v>912</v>
+        <v>905</v>
       </c>
       <c r="G297" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H297" s="2" t="s">
         <v>547</v>
@@ -11939,7 +11982,7 @@
         <v>153</v>
       </c>
       <c r="F298" s="11" t="s">
-        <v>841</v>
+        <v>834</v>
       </c>
       <c r="G298" s="21"/>
       <c r="H298" s="2" t="s">
@@ -11966,7 +12009,7 @@
         <v>154</v>
       </c>
       <c r="F299" s="11" t="s">
-        <v>842</v>
+        <v>835</v>
       </c>
       <c r="G299" s="21"/>
       <c r="H299" s="2" t="s">
@@ -11993,7 +12036,7 @@
         <v>413</v>
       </c>
       <c r="F300" s="2" t="s">
-        <v>843</v>
+        <v>836</v>
       </c>
       <c r="H300" s="2" t="s">
         <v>407</v>
@@ -12019,10 +12062,10 @@
         <v>622</v>
       </c>
       <c r="F301" s="9" t="s">
-        <v>913</v>
+        <v>906</v>
       </c>
       <c r="G301" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H301" s="2" t="s">
         <v>547</v>
@@ -12101,7 +12144,7 @@
         <v>423</v>
       </c>
       <c r="F304" s="11" t="s">
-        <v>845</v>
+        <v>838</v>
       </c>
       <c r="G304" s="21"/>
       <c r="H304" s="2" t="s">
@@ -12128,10 +12171,10 @@
         <v>605</v>
       </c>
       <c r="F305" s="9" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="G305" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H305" s="2" t="s">
         <v>352</v>
@@ -12157,7 +12200,7 @@
         <v>204</v>
       </c>
       <c r="F306" s="11" t="s">
-        <v>846</v>
+        <v>839</v>
       </c>
       <c r="G306" s="21"/>
       <c r="H306" s="2" t="s">
@@ -12184,7 +12227,7 @@
         <v>205</v>
       </c>
       <c r="F307" s="11" t="s">
-        <v>914</v>
+        <v>907</v>
       </c>
       <c r="H307" s="2" t="s">
         <v>120</v>
@@ -12210,10 +12253,10 @@
         <v>456</v>
       </c>
       <c r="F308" s="9" t="s">
-        <v>915</v>
+        <v>908</v>
       </c>
       <c r="G308" s="23" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H308" s="2" t="s">
         <v>429</v>
@@ -12239,7 +12282,7 @@
         <v>498</v>
       </c>
       <c r="F309" s="2" t="s">
-        <v>916</v>
+        <v>909</v>
       </c>
       <c r="H309" s="2" t="s">
         <v>416</v>
@@ -12265,10 +12308,10 @@
         <v>606</v>
       </c>
       <c r="F310" s="9" t="s">
-        <v>917</v>
+        <v>910</v>
       </c>
       <c r="G310" s="23" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H310" s="2" t="s">
         <v>352</v>
@@ -12294,10 +12337,10 @@
         <v>607</v>
       </c>
       <c r="F311" s="9" t="s">
-        <v>918</v>
+        <v>911</v>
       </c>
       <c r="G311" s="23" t="s">
-        <v>899</v>
+        <v>892</v>
       </c>
       <c r="H311" s="2" t="s">
         <v>352</v>
@@ -12323,10 +12366,10 @@
         <v>678</v>
       </c>
       <c r="F312" s="9" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="G312" s="23" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H312" s="2" t="s">
         <v>547</v>
@@ -12352,10 +12395,10 @@
         <v>680</v>
       </c>
       <c r="F313" s="9" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="G313" s="23" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H313" s="2" t="s">
         <v>547</v>
@@ -12381,10 +12424,10 @@
         <v>387</v>
       </c>
       <c r="F314" s="15" t="s">
-        <v>919</v>
+        <v>912</v>
       </c>
       <c r="G314" s="23" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H314" s="2" t="s">
         <v>369</v>
@@ -12410,7 +12453,7 @@
         <v>206</v>
       </c>
       <c r="F315" s="11" t="s">
-        <v>920</v>
+        <v>913</v>
       </c>
       <c r="H315" s="2" t="s">
         <v>120</v>
@@ -12436,7 +12479,7 @@
         <v>207</v>
       </c>
       <c r="F316" s="2" t="s">
-        <v>921</v>
+        <v>914</v>
       </c>
       <c r="H316" s="2" t="s">
         <v>120</v>
@@ -12462,7 +12505,7 @@
         <v>262</v>
       </c>
       <c r="F317" s="11" t="s">
-        <v>922</v>
+        <v>915</v>
       </c>
       <c r="H317" s="2" t="s">
         <v>248</v>
@@ -12488,7 +12531,7 @@
         <v>263</v>
       </c>
       <c r="F318" s="2" t="s">
-        <v>923</v>
+        <v>916</v>
       </c>
       <c r="H318" s="2" t="s">
         <v>248</v>
@@ -12514,10 +12557,10 @@
         <v>677</v>
       </c>
       <c r="F319" s="9" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="G319" s="23" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H319" s="2" t="s">
         <v>547</v>
@@ -12543,10 +12586,10 @@
         <v>676</v>
       </c>
       <c r="F320" s="9" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="G320" s="23" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H320" s="2" t="s">
         <v>547</v>
@@ -12572,10 +12615,10 @@
         <v>679</v>
       </c>
       <c r="F321" s="9" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="G321" s="23" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H321" s="2" t="s">
         <v>547</v>
@@ -12601,7 +12644,7 @@
         <v>457</v>
       </c>
       <c r="F322" s="11" t="s">
-        <v>857</v>
+        <v>850</v>
       </c>
       <c r="H322" s="2" t="s">
         <v>429</v>
@@ -12627,10 +12670,10 @@
         <v>458</v>
       </c>
       <c r="F323" s="9" t="s">
-        <v>924</v>
+        <v>917</v>
       </c>
       <c r="G323" s="23" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H323" s="2" t="s">
         <v>429</v>
@@ -12656,10 +12699,10 @@
         <v>499</v>
       </c>
       <c r="F324" s="9" t="s">
-        <v>925</v>
+        <v>918</v>
       </c>
       <c r="G324" s="23" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H324" s="2" t="s">
         <v>416</v>
@@ -12965,7 +13008,7 @@
         <v>412</v>
       </c>
       <c r="F337" s="16" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="H337" s="2" t="s">
         <v>407</v>
@@ -13014,7 +13057,7 @@
         <v>442</v>
       </c>
       <c r="F339" s="8" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="G339" s="19"/>
       <c r="H339" s="2" t="s">
@@ -13041,7 +13084,7 @@
         <v>538</v>
       </c>
       <c r="F340" s="11" t="s">
-        <v>849</v>
+        <v>842</v>
       </c>
       <c r="G340" s="21"/>
       <c r="H340" s="2" t="s">
@@ -13068,7 +13111,7 @@
         <v>536</v>
       </c>
       <c r="F341" s="11" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
       <c r="G341" s="21"/>
       <c r="H341" s="2" t="s">
@@ -13095,7 +13138,7 @@
         <v>537</v>
       </c>
       <c r="F342" s="11" t="s">
-        <v>851</v>
+        <v>844</v>
       </c>
       <c r="G342" s="21"/>
       <c r="H342" s="2" t="s">
@@ -13122,7 +13165,7 @@
         <v>226</v>
       </c>
       <c r="F343" s="11" t="s">
-        <v>852</v>
+        <v>845</v>
       </c>
       <c r="G343" s="21"/>
       <c r="H343" s="2" t="s">
@@ -13149,7 +13192,7 @@
         <v>227</v>
       </c>
       <c r="F344" s="11" t="s">
-        <v>853</v>
+        <v>846</v>
       </c>
       <c r="G344" s="21"/>
       <c r="H344" s="2" t="s">
@@ -13176,7 +13219,7 @@
         <v>228</v>
       </c>
       <c r="F345" s="11" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
       <c r="G345" s="21"/>
       <c r="H345" s="2" t="s">
@@ -13203,7 +13246,7 @@
         <v>411</v>
       </c>
       <c r="F346" s="2" t="s">
-        <v>855</v>
+        <v>848</v>
       </c>
       <c r="H346" s="2" t="s">
         <v>407</v>
@@ -13229,10 +13272,10 @@
         <v>500</v>
       </c>
       <c r="F347" s="9" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="G347" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H347" s="2" t="s">
         <v>416</v>
@@ -13258,10 +13301,10 @@
         <v>92</v>
       </c>
       <c r="F348" s="9" t="s">
-        <v>799</v>
+        <v>792</v>
       </c>
       <c r="G348" s="20" t="s">
-        <v>899</v>
+        <v>892</v>
       </c>
       <c r="H348" s="2" t="s">
         <v>85</v>
@@ -19359,13 +19402,13 @@
         <v>49</v>
       </c>
       <c r="E611" s="2" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="F611" s="9" t="s">
-        <v>796</v>
+        <v>789</v>
       </c>
       <c r="G611" s="20" t="s">
-        <v>905</v>
+        <v>898</v>
       </c>
       <c r="H611" s="2" t="s">
         <v>547</v>
@@ -19388,10 +19431,10 @@
         <v>45</v>
       </c>
       <c r="E612" s="2" t="s">
-        <v>879</v>
+        <v>872</v>
       </c>
       <c r="F612" s="11" t="s">
-        <v>827</v>
+        <v>820</v>
       </c>
       <c r="G612" s="21"/>
       <c r="H612" s="2" t="s">
@@ -19415,13 +19458,13 @@
         <v>46</v>
       </c>
       <c r="E613" s="2" t="s">
-        <v>844</v>
+        <v>837</v>
       </c>
       <c r="F613" s="9" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="G613" s="20" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="H613" s="2" t="s">
         <v>547</v>
@@ -19444,10 +19487,10 @@
         <v>45</v>
       </c>
       <c r="E614" s="2" t="s">
-        <v>880</v>
+        <v>873</v>
       </c>
       <c r="F614" s="11" t="s">
-        <v>881</v>
+        <v>874</v>
       </c>
       <c r="G614" s="21"/>
       <c r="H614" s="2" t="s">
@@ -19457,8 +19500,28 @@
         <v>708</v>
       </c>
     </row>
+    <row r="615" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C615" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D615" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E615" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="F615" s="11" t="s">
+        <v>927</v>
+      </c>
+      <c r="H615" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="I615" s="31" t="s">
+        <v>708</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:H614">
+  <autoFilter ref="B1:H615">
     <sortState ref="B2:H610">
       <sortCondition ref="H1:H610"/>
     </sortState>
@@ -19469,8 +19532,11 @@
     <sortCondition ref="D2:D610"/>
     <sortCondition ref="H2:H610"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="I615" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated color-coding based on resolutions
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@1305 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/ballots/2013-05 QA Review/FHIR May Results.xlsx
+++ b/ballots/2013-05 QA Review/FHIR May Results.xlsx
@@ -3090,9 +3090,6 @@
     <t>Provide guidance on use of name "recorder" vs. "author" - when appropriate for business usage</t>
   </si>
   <si>
-    <t>Provide guidance on use of name "type" vs. "code" - when appropriate for business usage</t>
-  </si>
-  <si>
     <t>Methodology discussion on correspondance between elements in "referenced" resources (subject, visit, etc.)</t>
   </si>
   <si>
@@ -3757,6 +3754,9 @@
   </si>
   <si>
     <t>#46 add a bit more documentation about this. There's now also a list of possible codes.</t>
+  </si>
+  <si>
+    <t>Provide guidance on use of name "type" vs. "code" - when appropriate for business usage - general guidance is to use "type", not "code".  Will update specs accordingly.</t>
   </si>
 </sst>
 </file>
@@ -4283,10 +4283,10 @@
   <dimension ref="A1:I622"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F64" sqref="F64"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4429,8 +4429,8 @@
       <c r="E5" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>954</v>
+      <c r="F5" s="11" t="s">
+        <v>953</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="2" t="s">
@@ -4483,11 +4483,11 @@
       <c r="E7" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>940</v>
+      <c r="F7" s="11" t="s">
+        <v>939</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>352</v>
@@ -4543,7 +4543,7 @@
         <v>741</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>547</v>
@@ -4598,7 +4598,7 @@
         <v>743</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>120</v>
@@ -4654,7 +4654,7 @@
         <v>745</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>407</v>
@@ -4709,7 +4709,7 @@
         <v>747</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>54</v>
@@ -4718,7 +4718,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -4734,11 +4734,11 @@
       <c r="E16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>748</v>
+      <c r="F16" s="11" t="s">
+        <v>957</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>54</v>
@@ -4764,10 +4764,10 @@
         <v>640</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>547</v>
@@ -4793,10 +4793,10 @@
         <v>482</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>416</v>
@@ -4822,7 +4822,7 @@
         <v>479</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>416</v>
@@ -4848,7 +4848,7 @@
         <v>478</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>416</v>
@@ -4874,10 +4874,10 @@
         <v>480</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>416</v>
@@ -4903,7 +4903,7 @@
         <v>481</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G22" s="18"/>
       <c r="H22" s="2" t="s">
@@ -4930,7 +4930,7 @@
         <v>483</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="2" t="s">
@@ -4945,7 +4945,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -4956,8 +4956,8 @@
       <c r="E24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>955</v>
+      <c r="F24" s="11" t="s">
+        <v>954</v>
       </c>
       <c r="G24" s="18"/>
       <c r="H24" s="2" t="s">
@@ -4972,7 +4972,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>6</v>
@@ -4998,7 +4998,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>6</v>
@@ -5010,7 +5010,7 @@
         <v>359</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>352</v>
@@ -5024,7 +5024,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>6</v>
@@ -5035,8 +5035,8 @@
       <c r="E27" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="F27" s="9" t="s">
-        <v>956</v>
+      <c r="F27" s="11" t="s">
+        <v>955</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="2" t="s">
@@ -5051,7 +5051,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>6</v>
@@ -5063,10 +5063,10 @@
         <v>380</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>369</v>
@@ -5080,7 +5080,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>6</v>
@@ -5092,7 +5092,7 @@
         <v>134</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>120</v>
@@ -5106,7 +5106,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>6</v>
@@ -5118,7 +5118,7 @@
         <v>254</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>248</v>
@@ -5132,7 +5132,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>6</v>
@@ -5144,7 +5144,7 @@
         <v>485</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>416</v>
@@ -5158,7 +5158,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>6</v>
@@ -5170,7 +5170,7 @@
         <v>484</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>416</v>
@@ -5184,7 +5184,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>6</v>
@@ -5196,7 +5196,7 @@
         <v>486</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>416</v>
@@ -5222,7 +5222,7 @@
         <v>64</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="2" t="s">
@@ -5276,7 +5276,7 @@
         <v>489</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="2" t="s">
@@ -5303,7 +5303,7 @@
         <v>487</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>352</v>
@@ -5329,7 +5329,7 @@
         <v>488</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="G38" s="20"/>
       <c r="H38" s="2" t="s">
@@ -5356,7 +5356,7 @@
         <v>490</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="2" t="s">
@@ -5383,7 +5383,7 @@
         <v>155</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="G40" s="20"/>
       <c r="H40" s="2" t="s">
@@ -5410,7 +5410,7 @@
         <v>417</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>416</v>
@@ -5435,11 +5435,11 @@
       <c r="E42" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F42" s="9" t="s">
-        <v>941</v>
+      <c r="F42" s="11" t="s">
+        <v>940</v>
       </c>
       <c r="G42" s="19" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>59</v>
@@ -5492,7 +5492,7 @@
         <v>491</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="G44" s="20"/>
       <c r="H44" s="2" t="s">
@@ -5519,7 +5519,7 @@
         <v>161</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G45" s="20"/>
       <c r="H45" s="2" t="s">
@@ -5546,7 +5546,7 @@
         <v>162</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="G46" s="20"/>
       <c r="H46" s="2" t="s">
@@ -5572,8 +5572,8 @@
       <c r="E47" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="F47" s="9" t="s">
-        <v>957</v>
+      <c r="F47" s="11" t="s">
+        <v>956</v>
       </c>
       <c r="G47" s="18"/>
       <c r="H47" s="2" t="s">
@@ -5600,7 +5600,7 @@
         <v>321</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G48" s="20"/>
       <c r="H48" s="2" t="s">
@@ -5627,7 +5627,7 @@
         <v>447</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G49" s="20"/>
       <c r="H49" s="2" t="s">
@@ -5654,7 +5654,7 @@
         <v>418</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>416</v>
@@ -5706,7 +5706,7 @@
         <v>514</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="G52" s="20"/>
       <c r="H52" s="2" t="s">
@@ -5733,7 +5733,7 @@
         <v>513</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="G53" s="20"/>
       <c r="H53" s="2" t="s">
@@ -5760,7 +5760,7 @@
         <v>163</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="G54" s="20"/>
       <c r="H54" s="2" t="s">
@@ -5787,7 +5787,7 @@
         <v>492</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="G55" s="20"/>
       <c r="H55" s="2" t="s">
@@ -5814,7 +5814,7 @@
         <v>71</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="G56" s="20"/>
       <c r="H56" s="2" t="s">
@@ -5870,7 +5870,7 @@
         <v>724</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>85</v>
@@ -5922,11 +5922,11 @@
       <c r="E60" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="F60" s="9" t="s">
-        <v>942</v>
+      <c r="F60" s="11" t="s">
+        <v>941</v>
       </c>
       <c r="G60" s="19" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>352</v>
@@ -5952,7 +5952,7 @@
         <v>516</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="G61" s="20"/>
       <c r="H61" s="2" t="s">
@@ -5979,7 +5979,7 @@
         <v>167</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="G62" s="20"/>
       <c r="H62" s="2" t="s">
@@ -6005,11 +6005,11 @@
       <c r="E63" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="F63" s="9" t="s">
-        <v>943</v>
+      <c r="F63" s="11" t="s">
+        <v>942</v>
       </c>
       <c r="G63" s="19" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>120</v>
@@ -6035,10 +6035,10 @@
         <v>169</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="G64" s="19" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>120</v>
@@ -6063,11 +6063,11 @@
       <c r="E65" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F65" s="9" t="s">
-        <v>945</v>
+      <c r="F65" s="11" t="s">
+        <v>944</v>
       </c>
       <c r="G65" s="19" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>120</v>
@@ -6093,7 +6093,7 @@
         <v>269</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="G66" s="18"/>
       <c r="H66" s="2" t="s">
@@ -6120,7 +6120,7 @@
         <v>418</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G67" s="20"/>
       <c r="H67" s="2" t="s">
@@ -6135,7 +6135,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>33</v>
@@ -6162,7 +6162,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>33</v>
@@ -6173,11 +6173,11 @@
       <c r="E69" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="F69" s="9" t="s">
-        <v>946</v>
+      <c r="F69" s="11" t="s">
+        <v>945</v>
       </c>
       <c r="G69" s="19" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>120</v>
@@ -6191,7 +6191,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>33</v>
@@ -6203,7 +6203,7 @@
         <v>209</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="G70" s="20"/>
       <c r="H70" s="2" t="s">
@@ -6218,7 +6218,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>33</v>
@@ -6230,7 +6230,7 @@
         <v>210</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="G71" s="20"/>
       <c r="H71" s="2" t="s">
@@ -6245,7 +6245,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>33</v>
@@ -6257,7 +6257,7 @@
         <v>211</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="G72" s="20"/>
       <c r="H72" s="2" t="s">
@@ -6272,7 +6272,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>33</v>
@@ -6284,7 +6284,7 @@
         <v>212</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="G73" s="20"/>
       <c r="H73" s="2" t="s">
@@ -6299,7 +6299,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>33</v>
@@ -6311,7 +6311,7 @@
         <v>459</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="G74" s="20"/>
       <c r="H74" s="2" t="s">
@@ -6326,7 +6326,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>33</v>
@@ -6338,7 +6338,7 @@
         <v>517</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>416</v>
@@ -6352,7 +6352,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>33</v>
@@ -6364,7 +6364,7 @@
         <v>518</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>416</v>
@@ -6389,8 +6389,8 @@
       <c r="E77" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="F77" s="9" t="s">
-        <v>947</v>
+      <c r="F77" s="11" t="s">
+        <v>946</v>
       </c>
       <c r="G77" s="19" t="s">
         <v>470</v>
@@ -6418,8 +6418,8 @@
       <c r="E78" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="F78" s="9" t="s">
-        <v>948</v>
+      <c r="F78" s="11" t="s">
+        <v>947</v>
       </c>
       <c r="G78" s="19" t="s">
         <v>470</v>
@@ -6447,11 +6447,11 @@
       <c r="E79" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="F79" s="9" t="s">
-        <v>949</v>
+      <c r="F79" s="11" t="s">
+        <v>948</v>
       </c>
       <c r="G79" s="19" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>85</v>
@@ -6528,8 +6528,8 @@
       <c r="E82" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="F82" s="9" t="s">
-        <v>950</v>
+      <c r="F82" s="11" t="s">
+        <v>949</v>
       </c>
       <c r="G82" s="19" t="s">
         <v>470</v>
@@ -6558,7 +6558,7 @@
         <v>683</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G83" s="20"/>
       <c r="H83" s="2" t="s">
@@ -6585,7 +6585,7 @@
         <v>684</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G84" s="20"/>
       <c r="H84" s="2" t="s">
@@ -6611,8 +6611,8 @@
       <c r="E85" s="2" t="s">
         <v>686</v>
       </c>
-      <c r="F85" s="9" t="s">
-        <v>951</v>
+      <c r="F85" s="11" t="s">
+        <v>950</v>
       </c>
       <c r="G85" s="19" t="s">
         <v>470</v>
@@ -6641,7 +6641,7 @@
         <v>688</v>
       </c>
       <c r="F86" s="16" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>547</v>
@@ -6667,7 +6667,7 @@
         <v>685</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>547</v>
@@ -6693,7 +6693,7 @@
         <v>382</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G88" s="27" t="s">
         <v>470</v>
@@ -6722,7 +6722,7 @@
         <v>383</v>
       </c>
       <c r="F89" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G89" s="25"/>
       <c r="H89" s="2" t="s">
@@ -6749,7 +6749,7 @@
         <v>384</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G90" s="25"/>
       <c r="H90" s="2" t="s">
@@ -6776,7 +6776,7 @@
         <v>385</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G91" s="25"/>
       <c r="H91" s="2" t="s">
@@ -6803,7 +6803,7 @@
         <v>386</v>
       </c>
       <c r="F92" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G92" s="25"/>
       <c r="H92" s="2" t="s">
@@ -6830,7 +6830,7 @@
         <v>214</v>
       </c>
       <c r="F93" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G93" s="20"/>
       <c r="H93" s="2" t="s">
@@ -6857,7 +6857,7 @@
         <v>215</v>
       </c>
       <c r="F94" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G94" s="20"/>
       <c r="H94" s="2" t="s">
@@ -6884,7 +6884,7 @@
         <v>216</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G95" s="20"/>
       <c r="H95" s="2" t="s">
@@ -6911,7 +6911,7 @@
         <v>217</v>
       </c>
       <c r="F96" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G96" s="20"/>
       <c r="H96" s="2" t="s">
@@ -6938,7 +6938,7 @@
         <v>218</v>
       </c>
       <c r="F97" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G97" s="20"/>
       <c r="H97" s="2" t="s">
@@ -6965,7 +6965,7 @@
         <v>219</v>
       </c>
       <c r="F98" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G98" s="20"/>
       <c r="H98" s="2" t="s">
@@ -6992,7 +6992,7 @@
         <v>220</v>
       </c>
       <c r="F99" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G99" s="20"/>
       <c r="H99" s="2" t="s">
@@ -7019,7 +7019,7 @@
         <v>221</v>
       </c>
       <c r="F100" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G100" s="20"/>
       <c r="H100" s="2" t="s">
@@ -7045,8 +7045,8 @@
       <c r="E101" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F101" s="9" t="s">
-        <v>952</v>
+      <c r="F101" s="11" t="s">
+        <v>951</v>
       </c>
       <c r="G101" s="19" t="s">
         <v>470</v>
@@ -7074,8 +7074,8 @@
       <c r="E102" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="F102" s="9" t="s">
-        <v>953</v>
+      <c r="F102" s="11" t="s">
+        <v>952</v>
       </c>
       <c r="G102" s="19" t="s">
         <v>470</v>
@@ -7104,7 +7104,7 @@
         <v>462</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="H103" s="2" t="s">
         <v>429</v>
@@ -7130,7 +7130,7 @@
         <v>519</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="H104" s="2" t="s">
         <v>416</v>
@@ -7156,7 +7156,7 @@
         <v>520</v>
       </c>
       <c r="F105" s="11" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="G105" s="20"/>
       <c r="H105" s="2" t="s">
@@ -7182,7 +7182,7 @@
       <c r="E106" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F106" s="8" t="s">
+      <c r="F106" s="9" t="s">
         <v>731</v>
       </c>
       <c r="G106" s="18"/>
@@ -7210,7 +7210,7 @@
         <v>599</v>
       </c>
       <c r="F107" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G107" s="20"/>
       <c r="H107" s="2" t="s">
@@ -7236,11 +7236,11 @@
       <c r="E108" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="F108" s="9" t="s">
-        <v>862</v>
+      <c r="F108" s="11" t="s">
+        <v>861</v>
       </c>
       <c r="G108" s="19" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="H108" s="2" t="s">
         <v>352</v>
@@ -7266,7 +7266,7 @@
         <v>583</v>
       </c>
       <c r="F109" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G109" s="20"/>
       <c r="H109" s="2" t="s">
@@ -7293,7 +7293,7 @@
         <v>587</v>
       </c>
       <c r="F110" s="11" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G110" s="20"/>
       <c r="H110" s="2" t="s">
@@ -7320,7 +7320,7 @@
         <v>405</v>
       </c>
       <c r="F111" s="14" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G111" s="25"/>
       <c r="H111" s="2" t="s">
@@ -7347,7 +7347,7 @@
         <v>137</v>
       </c>
       <c r="F112" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G112" s="20"/>
       <c r="H112" s="2" t="s">
@@ -7374,7 +7374,7 @@
         <v>138</v>
       </c>
       <c r="F113" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G113" s="20"/>
       <c r="H113" s="2" t="s">
@@ -7401,7 +7401,7 @@
         <v>139</v>
       </c>
       <c r="F114" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G114" s="20"/>
       <c r="H114" s="2" t="s">
@@ -7428,10 +7428,10 @@
         <v>590</v>
       </c>
       <c r="F115" s="9" t="s">
+        <v>880</v>
+      </c>
+      <c r="G115" s="19" t="s">
         <v>881</v>
-      </c>
-      <c r="G115" s="19" t="s">
-        <v>882</v>
       </c>
       <c r="H115" s="2" t="s">
         <v>547</v>
@@ -7457,7 +7457,7 @@
         <v>582</v>
       </c>
       <c r="F116" s="11" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G116" s="20"/>
       <c r="H116" s="2" t="s">
@@ -7484,7 +7484,7 @@
         <v>585</v>
       </c>
       <c r="F117" s="11" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G117" s="20"/>
       <c r="H117" s="2" t="s">
@@ -7511,7 +7511,7 @@
         <v>584</v>
       </c>
       <c r="F118" s="11" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G118" s="20"/>
       <c r="H118" s="2" t="s">
@@ -7538,7 +7538,7 @@
         <v>436</v>
       </c>
       <c r="F119" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G119" s="20"/>
       <c r="H119" s="2" t="s">
@@ -7565,7 +7565,7 @@
         <v>437</v>
       </c>
       <c r="F120" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G120" s="20"/>
       <c r="H120" s="2" t="s">
@@ -7592,7 +7592,7 @@
         <v>493</v>
       </c>
       <c r="F121" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G121" s="20"/>
       <c r="H121" s="2" t="s">
@@ -7619,7 +7619,7 @@
         <v>586</v>
       </c>
       <c r="F122" s="11" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="G122" s="20"/>
       <c r="H122" s="2" t="s">
@@ -7645,7 +7645,7 @@
       <c r="E123" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F123" s="9" t="s">
+      <c r="F123" s="11" t="s">
         <v>729</v>
       </c>
       <c r="G123" s="19" t="s">
@@ -7674,8 +7674,8 @@
       <c r="E124" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="F124" s="9" t="s">
-        <v>868</v>
+      <c r="F124" s="11" t="s">
+        <v>867</v>
       </c>
       <c r="G124" s="19" t="s">
         <v>8</v>
@@ -7703,8 +7703,8 @@
       <c r="E125" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="F125" s="9" t="s">
-        <v>869</v>
+      <c r="F125" s="11" t="s">
+        <v>868</v>
       </c>
       <c r="G125" s="19" t="s">
         <v>8</v>
@@ -7733,7 +7733,7 @@
         <v>404</v>
       </c>
       <c r="F126" s="13" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="G126" s="24"/>
       <c r="H126" s="2" t="s">
@@ -7760,7 +7760,7 @@
         <v>140</v>
       </c>
       <c r="F127" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G127" s="20"/>
       <c r="H127" s="2" t="s">
@@ -7787,7 +7787,7 @@
         <v>141</v>
       </c>
       <c r="F128" s="11" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="G128" s="20"/>
       <c r="H128" s="2" t="s">
@@ -7814,7 +7814,7 @@
         <v>142</v>
       </c>
       <c r="F129" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G129" s="20"/>
       <c r="H129" s="2" t="s">
@@ -7841,7 +7841,7 @@
         <v>143</v>
       </c>
       <c r="F130" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G130" s="20"/>
       <c r="H130" s="2" t="s">
@@ -7868,7 +7868,7 @@
         <v>258</v>
       </c>
       <c r="F131" s="11" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="G131" s="20"/>
       <c r="H131" s="2" t="s">
@@ -7895,7 +7895,7 @@
         <v>588</v>
       </c>
       <c r="F132" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G132" s="20"/>
       <c r="H132" s="2" t="s">
@@ -7922,7 +7922,7 @@
         <v>438</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G133" s="20"/>
       <c r="H133" s="2" t="s">
@@ -8020,7 +8020,7 @@
         <v>144</v>
       </c>
       <c r="F137" s="11" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G137" s="20"/>
       <c r="H137" s="2" t="s">
@@ -8237,7 +8237,7 @@
         <v>495</v>
       </c>
       <c r="F146" s="11" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="G146" s="20"/>
       <c r="H146" s="2" t="s">
@@ -8314,7 +8314,7 @@
         <v>156</v>
       </c>
       <c r="F149" s="11" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="G149" s="20"/>
       <c r="H149" s="2" t="s">
@@ -8341,7 +8341,7 @@
         <v>157</v>
       </c>
       <c r="F150" s="11" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="G150" s="20"/>
       <c r="H150" s="2" t="s">
@@ -8368,7 +8368,7 @@
         <v>158</v>
       </c>
       <c r="F151" s="11" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="G151" s="20"/>
       <c r="H151" s="2" t="s">
@@ -8464,7 +8464,7 @@
         <v>310</v>
       </c>
       <c r="F155" s="11" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="G155" s="20"/>
       <c r="H155" s="2" t="s">
@@ -8744,7 +8744,7 @@
         <v>445</v>
       </c>
       <c r="F167" s="11" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G167" s="20"/>
       <c r="H167" s="2" t="s">
@@ -8942,7 +8942,7 @@
         <v>733</v>
       </c>
       <c r="G175" s="19" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H175" s="2" t="s">
         <v>85</v>
@@ -9018,7 +9018,7 @@
         <v>388</v>
       </c>
       <c r="F178" s="14" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="G178" s="25"/>
       <c r="H178" s="2" t="s">
@@ -9137,7 +9137,7 @@
         <v>524</v>
       </c>
       <c r="F183" s="11" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G183" s="20"/>
       <c r="H183" s="2" t="s">
@@ -9164,7 +9164,7 @@
         <v>525</v>
       </c>
       <c r="F184" s="11" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G184" s="20"/>
       <c r="H184" s="2" t="s">
@@ -9191,7 +9191,7 @@
         <v>526</v>
       </c>
       <c r="F185" s="11" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G185" s="20"/>
       <c r="H185" s="2" t="s">
@@ -9358,7 +9358,7 @@
         <v>132</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="H192" s="2" t="s">
         <v>120</v>
@@ -9549,7 +9549,7 @@
         <v>247</v>
       </c>
       <c r="F200" s="11" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="G200" s="20"/>
       <c r="H200" s="2" t="s">
@@ -9741,7 +9741,7 @@
         <v>399</v>
       </c>
       <c r="F208" s="14" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G208" s="25"/>
       <c r="H208" s="2" t="s">
@@ -9768,7 +9768,7 @@
         <v>400</v>
       </c>
       <c r="F209" s="14" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G209" s="25"/>
       <c r="H209" s="2" t="s">
@@ -9795,7 +9795,7 @@
         <v>401</v>
       </c>
       <c r="F210" s="14" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="G210" s="25"/>
       <c r="H210" s="2" t="s">
@@ -9822,7 +9822,7 @@
         <v>402</v>
       </c>
       <c r="F211" s="4" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="G211" s="28"/>
       <c r="H211" s="2" t="s">
@@ -9918,7 +9918,7 @@
         <v>290</v>
       </c>
       <c r="F215" s="9" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="G215" s="19" t="s">
         <v>470</v>
@@ -10085,7 +10085,7 @@
         <v>297</v>
       </c>
       <c r="F222" s="8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="G222" s="18"/>
       <c r="H222" s="2" t="s">
@@ -10365,7 +10365,7 @@
         <v>443</v>
       </c>
       <c r="F234" s="11" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="G234" s="20"/>
       <c r="H234" s="2" t="s">
@@ -10415,7 +10415,7 @@
         <v>529</v>
       </c>
       <c r="F236" s="11" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="G236" s="20"/>
       <c r="H236" s="2" t="s">
@@ -10468,7 +10468,7 @@
         <v>736</v>
       </c>
       <c r="G238" s="19" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H238" s="2" t="s">
         <v>85</v>
@@ -10563,7 +10563,7 @@
         <v>460</v>
       </c>
       <c r="F242" s="11" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G242" s="20"/>
       <c r="H242" s="2" t="s">
@@ -10590,7 +10590,7 @@
         <v>461</v>
       </c>
       <c r="F243" s="8" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="G243" s="18"/>
       <c r="H243" s="2" t="s">
@@ -10640,7 +10640,7 @@
         <v>532</v>
       </c>
       <c r="F245" s="11" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="G245" s="20"/>
       <c r="H245" s="2" t="s">
@@ -10693,10 +10693,10 @@
         <v>223</v>
       </c>
       <c r="F247" s="9" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="G247" s="19" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H247" s="2" t="s">
         <v>120</v>
@@ -10768,7 +10768,7 @@
         <v>463</v>
       </c>
       <c r="F250" s="11" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="G250" s="20"/>
       <c r="H250" s="2" t="s">
@@ -10795,7 +10795,7 @@
         <v>534</v>
       </c>
       <c r="F251" s="11" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G251" s="20"/>
       <c r="H251" s="2" t="s">
@@ -10822,7 +10822,7 @@
         <v>533</v>
       </c>
       <c r="F252" s="11" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G252" s="20"/>
       <c r="H252" s="2" t="s">
@@ -10872,10 +10872,10 @@
         <v>60</v>
       </c>
       <c r="F254" s="11" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G254" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H254" s="2" t="s">
         <v>59</v>
@@ -10901,10 +10901,10 @@
         <v>249</v>
       </c>
       <c r="F255" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="G255" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H255" s="2" t="s">
         <v>248</v>
@@ -10930,10 +10930,10 @@
         <v>276</v>
       </c>
       <c r="F256" s="11" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="G256" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H256" s="2" t="s">
         <v>351</v>
@@ -10959,10 +10959,10 @@
         <v>278</v>
       </c>
       <c r="F257" s="9" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="G257" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H257" s="2" t="s">
         <v>351</v>
@@ -10988,10 +10988,10 @@
         <v>279</v>
       </c>
       <c r="F258" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="G258" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H258" s="2" t="s">
         <v>351</v>
@@ -11017,10 +11017,10 @@
         <v>372</v>
       </c>
       <c r="F259" s="13" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="G259" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H259" s="2" t="s">
         <v>369</v>
@@ -11046,10 +11046,10 @@
         <v>241</v>
       </c>
       <c r="F260" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="G260" s="19" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="H260" s="2" t="s">
         <v>238</v>
@@ -11075,10 +11075,10 @@
         <v>357</v>
       </c>
       <c r="F261" s="11" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="G261" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H261" s="2" t="s">
         <v>352</v>
@@ -11104,10 +11104,10 @@
         <v>621</v>
       </c>
       <c r="F262" s="11" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="G262" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H262" s="2" t="s">
         <v>547</v>
@@ -11133,10 +11133,10 @@
         <v>363</v>
       </c>
       <c r="F263" s="11" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="G263" s="19" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="H263" s="2" t="s">
         <v>352</v>
@@ -11162,10 +11162,10 @@
         <v>620</v>
       </c>
       <c r="F264" s="11" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="G264" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H264" s="2" t="s">
         <v>547</v>
@@ -11191,10 +11191,10 @@
         <v>622</v>
       </c>
       <c r="F265" s="11" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="G265" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H265" s="2" t="s">
         <v>547</v>
@@ -11220,10 +11220,10 @@
         <v>605</v>
       </c>
       <c r="F266" s="9" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="G266" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H266" s="2" t="s">
         <v>352</v>
@@ -11249,10 +11249,10 @@
         <v>456</v>
       </c>
       <c r="F267" s="11" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G267" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H267" s="2" t="s">
         <v>429</v>
@@ -11278,10 +11278,10 @@
         <v>606</v>
       </c>
       <c r="F268" s="11" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="G268" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H268" s="2" t="s">
         <v>352</v>
@@ -11307,10 +11307,10 @@
         <v>607</v>
       </c>
       <c r="F269" s="9" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="G269" s="22" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="H269" s="2" t="s">
         <v>352</v>
@@ -11336,10 +11336,10 @@
         <v>678</v>
       </c>
       <c r="F270" s="11" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="G270" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H270" s="2" t="s">
         <v>547</v>
@@ -11365,10 +11365,10 @@
         <v>680</v>
       </c>
       <c r="F271" s="11" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="G271" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H271" s="2" t="s">
         <v>547</v>
@@ -11394,10 +11394,10 @@
         <v>387</v>
       </c>
       <c r="F272" s="14" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="G272" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H272" s="2" t="s">
         <v>369</v>
@@ -11423,10 +11423,10 @@
         <v>677</v>
       </c>
       <c r="F273" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="G273" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H273" s="2" t="s">
         <v>547</v>
@@ -11452,10 +11452,10 @@
         <v>676</v>
       </c>
       <c r="F274" s="9" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="G274" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H274" s="2" t="s">
         <v>547</v>
@@ -11481,10 +11481,10 @@
         <v>679</v>
       </c>
       <c r="F275" s="9" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="G275" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H275" s="2" t="s">
         <v>547</v>
@@ -11510,10 +11510,10 @@
         <v>458</v>
       </c>
       <c r="F276" s="9" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="G276" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H276" s="2" t="s">
         <v>429</v>
@@ -11539,10 +11539,10 @@
         <v>499</v>
       </c>
       <c r="F277" s="9" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="G277" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H277" s="2" t="s">
         <v>416</v>
@@ -11594,7 +11594,7 @@
         <v>239</v>
       </c>
       <c r="F279" s="8" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="G279" s="18"/>
       <c r="H279" s="2" t="s">
@@ -11621,7 +11621,7 @@
         <v>355</v>
       </c>
       <c r="F280" s="2" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H280" s="2" t="s">
         <v>352</v>
@@ -11647,7 +11647,7 @@
         <v>231</v>
       </c>
       <c r="F281" s="2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="H281" s="2" t="s">
         <v>230</v>
@@ -11673,7 +11673,7 @@
         <v>370</v>
       </c>
       <c r="F282" s="2" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H282" s="2" t="s">
         <v>369</v>
@@ -11699,7 +11699,7 @@
         <v>371</v>
       </c>
       <c r="F283" s="14" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G283" s="25"/>
       <c r="H283" s="2" t="s">
@@ -11726,7 +11726,7 @@
         <v>123</v>
       </c>
       <c r="F284" s="11" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="G284" s="20"/>
       <c r="H284" s="2" t="s">
@@ -11753,7 +11753,7 @@
         <v>124</v>
       </c>
       <c r="F285" s="11" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="G285" s="20"/>
       <c r="H285" s="2" t="s">
@@ -11780,7 +11780,7 @@
         <v>250</v>
       </c>
       <c r="F286" s="2" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="H286" s="2" t="s">
         <v>248</v>
@@ -11806,7 +11806,7 @@
         <v>408</v>
       </c>
       <c r="F287" s="11" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="G287" s="20"/>
       <c r="H287" s="2" t="s">
@@ -11833,7 +11833,7 @@
         <v>277</v>
       </c>
       <c r="F288" s="11" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="G288" s="20"/>
       <c r="H288" s="2" t="s">
@@ -11860,7 +11860,7 @@
         <v>430</v>
       </c>
       <c r="F289" s="8" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G289" s="18"/>
       <c r="H289" s="2" t="s">
@@ -11887,7 +11887,7 @@
         <v>431</v>
       </c>
       <c r="F290" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="H290" s="2" t="s">
         <v>429</v>
@@ -11939,7 +11939,7 @@
         <v>232</v>
       </c>
       <c r="F292" s="2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="H292" s="2" t="s">
         <v>230</v>
@@ -11965,7 +11965,7 @@
         <v>373</v>
       </c>
       <c r="F293" s="4" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="G293" s="28"/>
       <c r="H293" s="2" t="s">
@@ -11992,7 +11992,7 @@
         <v>125</v>
       </c>
       <c r="F294" s="11" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="G294" s="20"/>
       <c r="H294" s="2" t="s">
@@ -12019,7 +12019,7 @@
         <v>126</v>
       </c>
       <c r="F295" s="11" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="G295" s="20"/>
       <c r="H295" s="2" t="s">
@@ -12046,7 +12046,7 @@
         <v>251</v>
       </c>
       <c r="F296" s="8" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="G296" s="18"/>
       <c r="H296" s="2" t="s">
@@ -12073,7 +12073,7 @@
         <v>432</v>
       </c>
       <c r="F297" s="8" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G297" s="18"/>
       <c r="H297" s="2" t="s">
@@ -12100,7 +12100,7 @@
         <v>433</v>
       </c>
       <c r="F298" s="11" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="G298" s="20"/>
       <c r="H298" s="2" t="s">
@@ -12127,7 +12127,7 @@
         <v>496</v>
       </c>
       <c r="F299" s="11" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="G299" s="20"/>
       <c r="H299" s="2" t="s">
@@ -12154,7 +12154,7 @@
         <v>61</v>
       </c>
       <c r="F300" s="8" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="G300" s="18"/>
       <c r="H300" s="2" t="s">
@@ -12181,7 +12181,7 @@
         <v>374</v>
       </c>
       <c r="F301" s="14" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="G301" s="25"/>
       <c r="H301" s="2" t="s">
@@ -12208,7 +12208,7 @@
         <v>375</v>
       </c>
       <c r="F302" s="4" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G302" s="28"/>
       <c r="H302" s="2" t="s">
@@ -12235,7 +12235,7 @@
         <v>376</v>
       </c>
       <c r="F303" s="14" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G303" s="25"/>
       <c r="H303" s="2" t="s">
@@ -12262,7 +12262,7 @@
         <v>127</v>
       </c>
       <c r="F304" s="11" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="G304" s="20"/>
       <c r="H304" s="2" t="s">
@@ -12289,7 +12289,7 @@
         <v>128</v>
       </c>
       <c r="F305" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="G305" s="20"/>
       <c r="H305" s="2" t="s">
@@ -12316,7 +12316,7 @@
         <v>129</v>
       </c>
       <c r="F306" s="11" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="G306" s="20"/>
       <c r="H306" s="2" t="s">
@@ -12343,7 +12343,7 @@
         <v>130</v>
       </c>
       <c r="F307" s="11" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="G307" s="20"/>
       <c r="H307" s="2" t="s">
@@ -12370,7 +12370,7 @@
         <v>409</v>
       </c>
       <c r="F308" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="H308" s="2" t="s">
         <v>407</v>
@@ -12396,7 +12396,7 @@
         <v>434</v>
       </c>
       <c r="F309" s="11" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="G309" s="20"/>
       <c r="H309" s="2" t="s">
@@ -12423,7 +12423,7 @@
         <v>497</v>
       </c>
       <c r="F310" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="H310" s="2" t="s">
         <v>416</v>
@@ -12449,7 +12449,7 @@
         <v>153</v>
       </c>
       <c r="F311" s="11" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="G311" s="20"/>
       <c r="H311" s="2" t="s">
@@ -12476,7 +12476,7 @@
         <v>154</v>
       </c>
       <c r="F312" s="11" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="G312" s="20"/>
       <c r="H312" s="2" t="s">
@@ -12503,7 +12503,7 @@
         <v>413</v>
       </c>
       <c r="F313" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H313" s="2" t="s">
         <v>407</v>
@@ -12529,7 +12529,7 @@
         <v>444</v>
       </c>
       <c r="F314" s="8" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G314" s="18"/>
       <c r="H314" s="2" t="s">
@@ -12582,7 +12582,7 @@
         <v>423</v>
       </c>
       <c r="F316" s="11" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G316" s="20"/>
       <c r="H316" s="2" t="s">
@@ -12609,7 +12609,7 @@
         <v>204</v>
       </c>
       <c r="F317" s="11" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="G317" s="20"/>
       <c r="H317" s="2" t="s">
@@ -12636,7 +12636,7 @@
         <v>205</v>
       </c>
       <c r="F318" s="11" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="H318" s="2" t="s">
         <v>120</v>
@@ -12662,7 +12662,7 @@
         <v>498</v>
       </c>
       <c r="F319" s="2" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="H319" s="2" t="s">
         <v>416</v>
@@ -12688,7 +12688,7 @@
         <v>206</v>
       </c>
       <c r="F320" s="11" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="H320" s="2" t="s">
         <v>120</v>
@@ -12714,7 +12714,7 @@
         <v>207</v>
       </c>
       <c r="F321" s="2" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="H321" s="2" t="s">
         <v>120</v>
@@ -12740,7 +12740,7 @@
         <v>262</v>
       </c>
       <c r="F322" s="11" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H322" s="2" t="s">
         <v>248</v>
@@ -12766,7 +12766,7 @@
         <v>263</v>
       </c>
       <c r="F323" s="2" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H323" s="2" t="s">
         <v>248</v>
@@ -12792,7 +12792,7 @@
         <v>457</v>
       </c>
       <c r="F324" s="11" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="H324" s="2" t="s">
         <v>429</v>
@@ -13098,7 +13098,7 @@
         <v>412</v>
       </c>
       <c r="F337" s="15" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H337" s="2" t="s">
         <v>407</v>
@@ -13147,7 +13147,7 @@
         <v>442</v>
       </c>
       <c r="F339" s="8" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="G339" s="18"/>
       <c r="H339" s="2" t="s">
@@ -13174,7 +13174,7 @@
         <v>538</v>
       </c>
       <c r="F340" s="11" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="G340" s="20"/>
       <c r="H340" s="2" t="s">
@@ -13201,7 +13201,7 @@
         <v>536</v>
       </c>
       <c r="F341" s="11" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G341" s="20"/>
       <c r="H341" s="2" t="s">
@@ -13228,7 +13228,7 @@
         <v>537</v>
       </c>
       <c r="F342" s="11" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="G342" s="20"/>
       <c r="H342" s="2" t="s">
@@ -13255,7 +13255,7 @@
         <v>226</v>
       </c>
       <c r="F343" s="11" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="G343" s="20"/>
       <c r="H343" s="2" t="s">
@@ -13282,7 +13282,7 @@
         <v>227</v>
       </c>
       <c r="F344" s="11" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="G344" s="20"/>
       <c r="H344" s="2" t="s">
@@ -13309,7 +13309,7 @@
         <v>228</v>
       </c>
       <c r="F345" s="11" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G345" s="20"/>
       <c r="H345" s="2" t="s">
@@ -13336,7 +13336,7 @@
         <v>411</v>
       </c>
       <c r="F346" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="H346" s="2" t="s">
         <v>407</v>
@@ -13362,10 +13362,10 @@
         <v>500</v>
       </c>
       <c r="F347" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="G347" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H347" s="2" t="s">
         <v>416</v>
@@ -13391,10 +13391,10 @@
         <v>92</v>
       </c>
       <c r="F348" s="9" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="G348" s="19" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="H348" s="2" t="s">
         <v>85</v>
@@ -19492,13 +19492,13 @@
         <v>49</v>
       </c>
       <c r="E611" s="2" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F611" s="9" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="G611" s="19" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H611" s="2" t="s">
         <v>547</v>
@@ -19521,10 +19521,10 @@
         <v>45</v>
       </c>
       <c r="E612" s="2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F612" s="11" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="G612" s="20"/>
       <c r="H612" s="2" t="s">
@@ -19548,13 +19548,13 @@
         <v>46</v>
       </c>
       <c r="E613" s="2" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F613" s="9" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="G613" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H613" s="2" t="s">
         <v>547</v>
@@ -19577,10 +19577,10 @@
         <v>45</v>
       </c>
       <c r="E614" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="F614" s="11" t="s">
         <v>854</v>
-      </c>
-      <c r="F614" s="11" t="s">
-        <v>855</v>
       </c>
       <c r="G614" s="20"/>
       <c r="H614" s="2" t="s">
@@ -19595,7 +19595,7 @@
         <v>614</v>
       </c>
       <c r="B615" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C615" s="2" t="s">
         <v>6</v>
@@ -19604,10 +19604,10 @@
         <v>45</v>
       </c>
       <c r="E615" s="2" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="F615" s="11" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H615" s="2" t="s">
         <v>547</v>
@@ -19630,10 +19630,10 @@
         <v>46</v>
       </c>
       <c r="E616" s="2" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="F616" s="9" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="H616" s="2" t="s">
         <v>547</v>
@@ -19656,10 +19656,10 @@
         <v>45</v>
       </c>
       <c r="E617" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="F617" s="11" t="s">
         <v>910</v>
-      </c>
-      <c r="F617" s="11" t="s">
-        <v>911</v>
       </c>
       <c r="H617" s="2" t="s">
         <v>547</v>
@@ -19670,39 +19670,39 @@
     </row>
     <row r="618" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="E618" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="F618" s="9" t="s">
         <v>919</v>
-      </c>
-      <c r="F618" s="9" t="s">
-        <v>920</v>
       </c>
     </row>
     <row r="619" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="F619" s="11" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="620" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E620" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="F620" s="11" t="s">
         <v>927</v>
-      </c>
-      <c r="F620" s="11" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="621" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F621" s="2" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="622" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E622" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="F622" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="G622" s="22" t="s">
         <v>934</v>
-      </c>
-      <c r="F622" s="2" t="s">
-        <v>936</v>
-      </c>
-      <c r="G622" s="22" t="s">
-        <v>935</v>
       </c>
     </row>
   </sheetData>
@@ -21193,17 +21193,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Categorized late-add QA items
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@1307 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/ballots/2013-05 QA Review/FHIR May Results.xlsx
+++ b/ballots/2013-05 QA Review/FHIR May Results.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Review Comments'!$B$1:$H$619</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Review Comments'!$B$1:$H$622</definedName>
     <definedName name="Resources">#REF!</definedName>
     <definedName name="Topics">#REF!</definedName>
   </definedNames>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4334" uniqueCount="958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4361" uniqueCount="960">
   <si>
     <t>Resource</t>
   </si>
@@ -3757,6 +3757,12 @@
   </si>
   <si>
     <t>Provide guidance on use of name "type" vs. "code" - when appropriate for business usage - general guidance is to use "type", not "code".  Will update specs accordingly.</t>
+  </si>
+  <si>
+    <t>No.  Change to a single "editor"</t>
+  </si>
+  <si>
+    <t>Need a place to capture family history information that can't be attributed to a single relative</t>
   </si>
 </sst>
 </file>
@@ -4283,10 +4289,10 @@
   <dimension ref="A1:I622"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E256" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="E257" sqref="E257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19668,45 +19674,141 @@
         <v>708</v>
       </c>
     </row>
-    <row r="618" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A618" s="2">
+        <v>617</v>
+      </c>
+      <c r="B618" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C618" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D618" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="E618" s="2" t="s">
         <v>918</v>
       </c>
       <c r="F618" s="9" t="s">
         <v>919</v>
       </c>
-    </row>
-    <row r="619" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H618" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="I618" s="2" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="619" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A619" s="2">
+        <v>618</v>
+      </c>
+      <c r="B619" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C619" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D619" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E619" s="2" t="s">
+        <v>959</v>
+      </c>
       <c r="F619" s="11" t="s">
         <v>921</v>
       </c>
+      <c r="H619" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="I619" s="2" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="620" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A620" s="2">
+        <v>619</v>
+      </c>
+      <c r="B620" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C620" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D620" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E620" s="2" t="s">
         <v>926</v>
       </c>
       <c r="F620" s="11" t="s">
         <v>927</v>
       </c>
+      <c r="H620" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="I620" s="2" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="621" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F621" s="2" t="s">
+      <c r="A621" s="2">
+        <v>620</v>
+      </c>
+      <c r="B621" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C621" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D621" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E621" s="2" t="s">
         <v>929</v>
       </c>
+      <c r="F621" s="11" t="s">
+        <v>958</v>
+      </c>
+      <c r="H621" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="I621" s="2" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="622" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A622" s="2">
+        <v>621</v>
+      </c>
+      <c r="B622" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C622" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D622" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="E622" s="2" t="s">
         <v>933</v>
       </c>
-      <c r="F622" s="2" t="s">
+      <c r="F622" s="9" t="s">
         <v>935</v>
       </c>
       <c r="G622" s="22" t="s">
         <v>934</v>
       </c>
+      <c r="H622" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="I622" s="2" t="s">
+        <v>708</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:H619">
+  <autoFilter ref="B1:H622">
     <filterColumn colId="0">
       <filters>
         <filter val="Core"/>

</xml_diff>